<commit_message>
Added due date and fixed how it was being imported
</commit_message>
<xml_diff>
--- a/material.xlsx
+++ b/material.xlsx
@@ -773,7 +773,7 @@
         <v>2502</v>
       </c>
       <c r="H6">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I6" t="s">
         <v>62</v>
@@ -806,7 +806,7 @@
         <v>69</v>
       </c>
       <c r="U6">
-        <v>73440</v>
+        <v>44880</v>
       </c>
       <c r="X6" s="1">
         <v>45720</v>

</xml_diff>